<commit_message>
update the latest Visualization file.
Moved file location from Source/Beta/Experiments to Reports Folder.
</commit_message>
<xml_diff>
--- a/Reports/jobspersalary.xlsx
+++ b/Reports/jobspersalary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tam\OneDrive\Documents\GitHub\PythonScrapJob\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tranc\OneDrive\Documents\GitHub\PythonScrapJob\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="12315"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Data Scientist</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Jobs Name</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -359,11 +356,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -374,117 +369,38 @@
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>1350</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <f>(1350*2+517)/3</f>
+        <v>1072.3333333333333</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>1350</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <f>MEDIAN(388,647)</f>
-        <v>517.5</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>1350</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>755</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>603.83000000000004</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>1186</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
+        <f>(755*2+603.83+1186)/5</f>
+        <v>659.96600000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>